<commit_message>
Added more progression charts
</commit_message>
<xml_diff>
--- a/progress_chart.xlsx
+++ b/progress_chart.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jaime\Desktop\git-repo\excel_examples\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1502A9C7-83EC-4C45-97FE-BA90BC5C8C18}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C900468A-7883-429D-922C-75FAE3D39292}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="810" yWindow="-120" windowWidth="28110" windowHeight="16440" xr2:uid="{85307BCC-6A82-4A39-9FF2-91306545CEFB}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>service</t>
   </si>
@@ -47,6 +47,15 @@
   </si>
   <si>
     <t>Difference</t>
+  </si>
+  <si>
+    <t>X</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>Labels</t>
   </si>
 </sst>
 </file>
@@ -96,12 +105,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="9" fontId="0" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="9" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -109,6 +125,12 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FF6816BA"/>
+      <color rgb="FFBE93FD"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -200,10 +222,10 @@
                 <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>0.67</c:v>
+                  <c:v>0.78</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.32999999999999996</c:v>
+                  <c:v>0.21999999999999997</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -312,6 +334,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000001-3F7C-4C1E-95C8-96DECF5D036F}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="1"/>
@@ -323,6 +350,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000003-3F7C-4C1E-95C8-96DECF5D036F}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="2"/>
@@ -334,6 +366,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000005-3F7C-4C1E-95C8-96DECF5D036F}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="3"/>
@@ -345,6 +382,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000007-3F7C-4C1E-95C8-96DECF5D036F}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="4"/>
@@ -356,6 +398,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000009-3F7C-4C1E-95C8-96DECF5D036F}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="5"/>
@@ -367,6 +414,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000000B-3F7C-4C1E-95C8-96DECF5D036F}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="6"/>
@@ -378,6 +430,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000000D-3F7C-4C1E-95C8-96DECF5D036F}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="7"/>
@@ -389,6 +446,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000000F-3F7C-4C1E-95C8-96DECF5D036F}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="8"/>
@@ -400,6 +462,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000011-3F7C-4C1E-95C8-96DECF5D036F}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="9"/>
@@ -411,6 +478,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000013-3F7C-4C1E-95C8-96DECF5D036F}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="10"/>
@@ -422,6 +494,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000015-3F7C-4C1E-95C8-96DECF5D036F}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="11"/>
@@ -433,6 +510,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000017-3F7C-4C1E-95C8-96DECF5D036F}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="12"/>
@@ -444,6 +526,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000019-3F7C-4C1E-95C8-96DECF5D036F}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="13"/>
@@ -455,6 +542,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000001B-3F7C-4C1E-95C8-96DECF5D036F}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="14"/>
@@ -466,6 +558,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000001D-3F7C-4C1E-95C8-96DECF5D036F}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="15"/>
@@ -477,6 +574,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000001F-3F7C-4C1E-95C8-96DECF5D036F}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="16"/>
@@ -488,6 +590,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000021-3F7C-4C1E-95C8-96DECF5D036F}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="17"/>
@@ -499,6 +606,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000023-3F7C-4C1E-95C8-96DECF5D036F}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="18"/>
@@ -510,6 +622,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000025-3F7C-4C1E-95C8-96DECF5D036F}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="19"/>
@@ -521,6 +638,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000027-3F7C-4C1E-95C8-96DECF5D036F}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:val>
             <c:numLit>
@@ -611,6 +733,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000029-3F7C-4C1E-95C8-96DECF5D036F}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="1"/>
@@ -640,10 +767,10 @@
                 <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>0.67</c:v>
+                  <c:v>0.78</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.32999999999999996</c:v>
+                  <c:v>0.21999999999999997</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -763,6 +890,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000001-8C9C-4F6F-AD22-8E79A37E2223}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="1"/>
@@ -780,6 +912,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000003-8C9C-4F6F-AD22-8E79A37E2223}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="2"/>
@@ -797,6 +934,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000005-8C9C-4F6F-AD22-8E79A37E2223}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="3"/>
@@ -814,6 +956,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000007-8C9C-4F6F-AD22-8E79A37E2223}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="4"/>
@@ -831,6 +978,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000009-8C9C-4F6F-AD22-8E79A37E2223}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="5"/>
@@ -848,6 +1000,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000000B-8C9C-4F6F-AD22-8E79A37E2223}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="6"/>
@@ -865,6 +1022,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000000D-8C9C-4F6F-AD22-8E79A37E2223}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="7"/>
@@ -882,6 +1044,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000000F-8C9C-4F6F-AD22-8E79A37E2223}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="8"/>
@@ -899,6 +1066,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000011-8C9C-4F6F-AD22-8E79A37E2223}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="9"/>
@@ -916,6 +1088,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000013-8C9C-4F6F-AD22-8E79A37E2223}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="10"/>
@@ -933,6 +1110,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000015-8C9C-4F6F-AD22-8E79A37E2223}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="11"/>
@@ -950,6 +1132,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000017-8C9C-4F6F-AD22-8E79A37E2223}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="12"/>
@@ -967,6 +1154,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000019-8C9C-4F6F-AD22-8E79A37E2223}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="13"/>
@@ -984,6 +1176,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000001B-8C9C-4F6F-AD22-8E79A37E2223}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="14"/>
@@ -1001,6 +1198,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000001D-8C9C-4F6F-AD22-8E79A37E2223}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="15"/>
@@ -1018,6 +1220,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000001F-8C9C-4F6F-AD22-8E79A37E2223}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="16"/>
@@ -1035,6 +1242,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000021-8C9C-4F6F-AD22-8E79A37E2223}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="17"/>
@@ -1052,6 +1264,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000023-8C9C-4F6F-AD22-8E79A37E2223}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="18"/>
@@ -1069,6 +1286,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000025-8C9C-4F6F-AD22-8E79A37E2223}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="19"/>
@@ -1086,6 +1308,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000027-8C9C-4F6F-AD22-8E79A37E2223}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="20"/>
@@ -1103,6 +1330,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000029-8C9C-4F6F-AD22-8E79A37E2223}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="21"/>
@@ -1120,6 +1352,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000002B-8C9C-4F6F-AD22-8E79A37E2223}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="22"/>
@@ -1137,6 +1374,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000002D-8C9C-4F6F-AD22-8E79A37E2223}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="23"/>
@@ -1154,6 +1396,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000002F-8C9C-4F6F-AD22-8E79A37E2223}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="24"/>
@@ -1171,6 +1418,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000031-8C9C-4F6F-AD22-8E79A37E2223}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="25"/>
@@ -1188,6 +1440,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000033-8C9C-4F6F-AD22-8E79A37E2223}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="26"/>
@@ -1205,6 +1462,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000035-8C9C-4F6F-AD22-8E79A37E2223}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="27"/>
@@ -1222,6 +1484,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000037-8C9C-4F6F-AD22-8E79A37E2223}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="28"/>
@@ -1239,6 +1506,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000039-8C9C-4F6F-AD22-8E79A37E2223}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="29"/>
@@ -1256,6 +1528,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000003B-8C9C-4F6F-AD22-8E79A37E2223}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="30"/>
@@ -1273,6 +1550,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000003D-8C9C-4F6F-AD22-8E79A37E2223}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="31"/>
@@ -1290,6 +1572,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000003F-8C9C-4F6F-AD22-8E79A37E2223}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="32"/>
@@ -1307,6 +1594,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000041-8C9C-4F6F-AD22-8E79A37E2223}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="33"/>
@@ -1324,6 +1616,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000043-8C9C-4F6F-AD22-8E79A37E2223}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="34"/>
@@ -1341,6 +1638,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000045-8C9C-4F6F-AD22-8E79A37E2223}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="35"/>
@@ -1358,6 +1660,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000047-8C9C-4F6F-AD22-8E79A37E2223}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="36"/>
@@ -1375,6 +1682,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000049-8C9C-4F6F-AD22-8E79A37E2223}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="37"/>
@@ -1392,6 +1704,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000004B-8C9C-4F6F-AD22-8E79A37E2223}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="38"/>
@@ -1409,6 +1726,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000004D-8C9C-4F6F-AD22-8E79A37E2223}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="39"/>
@@ -1426,6 +1748,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000004F-8C9C-4F6F-AD22-8E79A37E2223}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="40"/>
@@ -1443,6 +1770,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000051-8C9C-4F6F-AD22-8E79A37E2223}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="41"/>
@@ -1460,6 +1792,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000053-8C9C-4F6F-AD22-8E79A37E2223}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="42"/>
@@ -1477,6 +1814,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000055-8C9C-4F6F-AD22-8E79A37E2223}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="43"/>
@@ -1494,6 +1836,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000057-8C9C-4F6F-AD22-8E79A37E2223}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="44"/>
@@ -1511,6 +1858,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000059-8C9C-4F6F-AD22-8E79A37E2223}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="45"/>
@@ -1528,6 +1880,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000005B-8C9C-4F6F-AD22-8E79A37E2223}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="46"/>
@@ -1545,6 +1902,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000005D-8C9C-4F6F-AD22-8E79A37E2223}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="47"/>
@@ -1562,6 +1924,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000005F-8C9C-4F6F-AD22-8E79A37E2223}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="48"/>
@@ -1579,6 +1946,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000061-8C9C-4F6F-AD22-8E79A37E2223}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="49"/>
@@ -1596,6 +1968,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000063-8C9C-4F6F-AD22-8E79A37E2223}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:val>
             <c:numLit>
@@ -1937,10 +2314,10 @@
                 <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>0.67</c:v>
+                  <c:v>0.78</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.32999999999999996</c:v>
+                  <c:v>0.21999999999999997</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2055,6 +2432,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000001-24F3-44E9-A13E-44BFC16F4848}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="1"/>
@@ -2072,6 +2454,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000003-24F3-44E9-A13E-44BFC16F4848}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="2"/>
@@ -2089,6 +2476,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000005-24F3-44E9-A13E-44BFC16F4848}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="3"/>
@@ -2106,6 +2498,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000007-24F3-44E9-A13E-44BFC16F4848}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="4"/>
@@ -2123,6 +2520,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000009-24F3-44E9-A13E-44BFC16F4848}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="5"/>
@@ -2140,6 +2542,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000000B-24F3-44E9-A13E-44BFC16F4848}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="6"/>
@@ -2157,6 +2564,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000000D-24F3-44E9-A13E-44BFC16F4848}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="7"/>
@@ -2174,6 +2586,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000000F-24F3-44E9-A13E-44BFC16F4848}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="8"/>
@@ -2191,6 +2608,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000011-24F3-44E9-A13E-44BFC16F4848}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="9"/>
@@ -2208,6 +2630,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000013-24F3-44E9-A13E-44BFC16F4848}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="10"/>
@@ -2225,6 +2652,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000015-24F3-44E9-A13E-44BFC16F4848}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="11"/>
@@ -2242,6 +2674,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000017-24F3-44E9-A13E-44BFC16F4848}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="12"/>
@@ -2259,6 +2696,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000019-24F3-44E9-A13E-44BFC16F4848}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="13"/>
@@ -2276,6 +2718,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000001B-24F3-44E9-A13E-44BFC16F4848}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="14"/>
@@ -2293,6 +2740,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000001D-24F3-44E9-A13E-44BFC16F4848}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="15"/>
@@ -2310,6 +2762,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000001F-24F3-44E9-A13E-44BFC16F4848}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="16"/>
@@ -2327,6 +2784,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000021-24F3-44E9-A13E-44BFC16F4848}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="17"/>
@@ -2344,6 +2806,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000023-24F3-44E9-A13E-44BFC16F4848}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="18"/>
@@ -2361,6 +2828,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000025-24F3-44E9-A13E-44BFC16F4848}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="19"/>
@@ -2378,6 +2850,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000027-24F3-44E9-A13E-44BFC16F4848}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:val>
             <c:numLit>
@@ -2513,10 +2990,10 @@
                 <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>0.67</c:v>
+                  <c:v>0.78</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.32999999999999996</c:v>
+                  <c:v>0.21999999999999997</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2685,6 +3162,11 @@
                 </a:glow>
               </a:effectLst>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000001-8C3E-4234-AD22-24169CCD2DA4}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="1"/>
@@ -2722,6 +3204,11 @@
                 </a:glow>
               </a:effectLst>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000003-8C3E-4234-AD22-24169CCD2DA4}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="2"/>
@@ -2759,6 +3246,11 @@
                 </a:glow>
               </a:effectLst>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000005-8C3E-4234-AD22-24169CCD2DA4}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="3"/>
@@ -2796,6 +3288,11 @@
                 </a:glow>
               </a:effectLst>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000007-8C3E-4234-AD22-24169CCD2DA4}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="4"/>
@@ -2833,6 +3330,11 @@
                 </a:glow>
               </a:effectLst>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000009-8C3E-4234-AD22-24169CCD2DA4}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="5"/>
@@ -2870,6 +3372,11 @@
                 </a:glow>
               </a:effectLst>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000000B-8C3E-4234-AD22-24169CCD2DA4}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="6"/>
@@ -2907,6 +3414,11 @@
                 </a:glow>
               </a:effectLst>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000000D-8C3E-4234-AD22-24169CCD2DA4}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="7"/>
@@ -2944,6 +3456,11 @@
                 </a:glow>
               </a:effectLst>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000000F-8C3E-4234-AD22-24169CCD2DA4}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="8"/>
@@ -2981,6 +3498,11 @@
                 </a:glow>
               </a:effectLst>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000011-8C3E-4234-AD22-24169CCD2DA4}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="9"/>
@@ -3018,6 +3540,11 @@
                 </a:glow>
               </a:effectLst>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000013-8C3E-4234-AD22-24169CCD2DA4}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="10"/>
@@ -3055,6 +3582,11 @@
                 </a:glow>
               </a:effectLst>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000015-8C3E-4234-AD22-24169CCD2DA4}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="11"/>
@@ -3092,6 +3624,11 @@
                 </a:glow>
               </a:effectLst>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000017-8C3E-4234-AD22-24169CCD2DA4}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="12"/>
@@ -3129,6 +3666,11 @@
                 </a:glow>
               </a:effectLst>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000019-8C3E-4234-AD22-24169CCD2DA4}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="13"/>
@@ -3166,6 +3708,11 @@
                 </a:glow>
               </a:effectLst>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000001B-8C3E-4234-AD22-24169CCD2DA4}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="14"/>
@@ -3203,6 +3750,11 @@
                 </a:glow>
               </a:effectLst>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000001D-8C3E-4234-AD22-24169CCD2DA4}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="15"/>
@@ -3240,6 +3792,11 @@
                 </a:glow>
               </a:effectLst>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000001F-8C3E-4234-AD22-24169CCD2DA4}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="16"/>
@@ -3277,6 +3834,11 @@
                 </a:glow>
               </a:effectLst>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000021-8C3E-4234-AD22-24169CCD2DA4}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="17"/>
@@ -3314,6 +3876,11 @@
                 </a:glow>
               </a:effectLst>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000023-8C3E-4234-AD22-24169CCD2DA4}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="18"/>
@@ -3351,6 +3918,11 @@
                 </a:glow>
               </a:effectLst>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000025-8C3E-4234-AD22-24169CCD2DA4}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="19"/>
@@ -3388,6 +3960,11 @@
                 </a:glow>
               </a:effectLst>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000027-8C3E-4234-AD22-24169CCD2DA4}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="20"/>
@@ -3425,6 +4002,11 @@
                 </a:glow>
               </a:effectLst>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000029-8C3E-4234-AD22-24169CCD2DA4}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="21"/>
@@ -3462,6 +4044,11 @@
                 </a:glow>
               </a:effectLst>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000002B-8C3E-4234-AD22-24169CCD2DA4}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="22"/>
@@ -3499,6 +4086,11 @@
                 </a:glow>
               </a:effectLst>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000002D-8C3E-4234-AD22-24169CCD2DA4}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="23"/>
@@ -3536,6 +4128,11 @@
                 </a:glow>
               </a:effectLst>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000002F-8C3E-4234-AD22-24169CCD2DA4}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="24"/>
@@ -3573,6 +4170,11 @@
                 </a:glow>
               </a:effectLst>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000031-8C3E-4234-AD22-24169CCD2DA4}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="25"/>
@@ -3610,6 +4212,11 @@
                 </a:glow>
               </a:effectLst>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000033-8C3E-4234-AD22-24169CCD2DA4}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="26"/>
@@ -3647,6 +4254,11 @@
                 </a:glow>
               </a:effectLst>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000035-8C3E-4234-AD22-24169CCD2DA4}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="27"/>
@@ -3684,6 +4296,11 @@
                 </a:glow>
               </a:effectLst>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000037-8C3E-4234-AD22-24169CCD2DA4}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="28"/>
@@ -3721,6 +4338,11 @@
                 </a:glow>
               </a:effectLst>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000039-8C3E-4234-AD22-24169CCD2DA4}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="29"/>
@@ -3758,6 +4380,11 @@
                 </a:glow>
               </a:effectLst>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000003B-8C3E-4234-AD22-24169CCD2DA4}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="30"/>
@@ -3795,6 +4422,11 @@
                 </a:glow>
               </a:effectLst>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000003D-8C3E-4234-AD22-24169CCD2DA4}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="31"/>
@@ -3832,6 +4464,11 @@
                 </a:glow>
               </a:effectLst>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000003F-8C3E-4234-AD22-24169CCD2DA4}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="32"/>
@@ -3869,6 +4506,11 @@
                 </a:glow>
               </a:effectLst>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000041-8C3E-4234-AD22-24169CCD2DA4}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="33"/>
@@ -3906,6 +4548,11 @@
                 </a:glow>
               </a:effectLst>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000043-8C3E-4234-AD22-24169CCD2DA4}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="34"/>
@@ -3943,6 +4590,11 @@
                 </a:glow>
               </a:effectLst>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000045-8C3E-4234-AD22-24169CCD2DA4}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="35"/>
@@ -3980,6 +4632,11 @@
                 </a:glow>
               </a:effectLst>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000047-8C3E-4234-AD22-24169CCD2DA4}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="36"/>
@@ -4017,6 +4674,11 @@
                 </a:glow>
               </a:effectLst>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000049-8C3E-4234-AD22-24169CCD2DA4}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="37"/>
@@ -4054,6 +4716,11 @@
                 </a:glow>
               </a:effectLst>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000004B-8C3E-4234-AD22-24169CCD2DA4}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="38"/>
@@ -4091,6 +4758,11 @@
                 </a:glow>
               </a:effectLst>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000004D-8C3E-4234-AD22-24169CCD2DA4}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="39"/>
@@ -4128,6 +4800,11 @@
                 </a:glow>
               </a:effectLst>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000004F-8C3E-4234-AD22-24169CCD2DA4}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="40"/>
@@ -4165,6 +4842,11 @@
                 </a:glow>
               </a:effectLst>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000051-8C3E-4234-AD22-24169CCD2DA4}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="41"/>
@@ -4202,6 +4884,11 @@
                 </a:glow>
               </a:effectLst>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000053-8C3E-4234-AD22-24169CCD2DA4}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="42"/>
@@ -4239,6 +4926,11 @@
                 </a:glow>
               </a:effectLst>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000055-8C3E-4234-AD22-24169CCD2DA4}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="43"/>
@@ -4276,6 +4968,11 @@
                 </a:glow>
               </a:effectLst>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000057-8C3E-4234-AD22-24169CCD2DA4}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="44"/>
@@ -4313,6 +5010,11 @@
                 </a:glow>
               </a:effectLst>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000059-8C3E-4234-AD22-24169CCD2DA4}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="45"/>
@@ -4350,6 +5052,11 @@
                 </a:glow>
               </a:effectLst>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000005B-8C3E-4234-AD22-24169CCD2DA4}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="46"/>
@@ -4387,6 +5094,11 @@
                 </a:glow>
               </a:effectLst>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000005D-8C3E-4234-AD22-24169CCD2DA4}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="47"/>
@@ -4424,6 +5136,11 @@
                 </a:glow>
               </a:effectLst>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000005F-8C3E-4234-AD22-24169CCD2DA4}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="48"/>
@@ -4461,6 +5178,11 @@
                 </a:glow>
               </a:effectLst>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000061-8C3E-4234-AD22-24169CCD2DA4}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="49"/>
@@ -4498,6 +5220,11 @@
                 </a:glow>
               </a:effectLst>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000063-8C3E-4234-AD22-24169CCD2DA4}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:val>
             <c:numLit>
@@ -4726,10 +5453,10 @@
                 <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>0.67</c:v>
+                  <c:v>0.78</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.32999999999999996</c:v>
+                  <c:v>0.21999999999999997</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4918,7 +5645,7 @@
                 <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>0.67</c:v>
+                  <c:v>0.78</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4999,7 +5726,7 @@
                 <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>0.32999999999999996</c:v>
+                  <c:v>0.21999999999999997</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5083,6 +5810,2161 @@
   </c:chart>
   <c:spPr>
     <a:noFill/>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:doughnutChart>
+        <c:varyColors val="1"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>breakdown</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:gradFill flip="none" rotWithShape="1">
+              <a:gsLst>
+                <a:gs pos="20000">
+                  <a:schemeClr val="accent5">
+                    <a:lumMod val="60000"/>
+                    <a:lumOff val="40000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="70000">
+                  <a:schemeClr val="accent5">
+                    <a:lumMod val="75000"/>
+                  </a:schemeClr>
+                </a:gs>
+              </a:gsLst>
+              <a:lin ang="10800000" scaled="1"/>
+              <a:tileRect/>
+            </a:gradFill>
+            <a:ln w="95250">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:gradFill flip="none" rotWithShape="1">
+                <a:gsLst>
+                  <a:gs pos="20000">
+                    <a:schemeClr val="accent5">
+                      <a:lumMod val="60000"/>
+                      <a:lumOff val="40000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="70000">
+                    <a:schemeClr val="accent5">
+                      <a:lumMod val="75000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="10800000" scaled="1"/>
+                <a:tileRect/>
+              </a:gradFill>
+              <a:ln w="95250">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="1"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:gradFill flip="none" rotWithShape="1">
+                <a:gsLst>
+                  <a:gs pos="20000">
+                    <a:schemeClr val="accent5">
+                      <a:lumMod val="60000"/>
+                      <a:lumOff val="40000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="70000">
+                    <a:schemeClr val="accent5">
+                      <a:lumMod val="75000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="10800000" scaled="1"/>
+                <a:tileRect/>
+              </a:gradFill>
+              <a:ln w="95250">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="2"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:gradFill flip="none" rotWithShape="1">
+                <a:gsLst>
+                  <a:gs pos="20000">
+                    <a:schemeClr val="accent5">
+                      <a:lumMod val="60000"/>
+                      <a:lumOff val="40000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="70000">
+                    <a:schemeClr val="accent5">
+                      <a:lumMod val="75000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="10800000" scaled="1"/>
+                <a:tileRect/>
+              </a:gradFill>
+              <a:ln w="95250">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="3"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:gradFill flip="none" rotWithShape="1">
+                <a:gsLst>
+                  <a:gs pos="20000">
+                    <a:schemeClr val="accent5">
+                      <a:lumMod val="60000"/>
+                      <a:lumOff val="40000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="70000">
+                    <a:schemeClr val="accent5">
+                      <a:lumMod val="75000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="10800000" scaled="1"/>
+                <a:tileRect/>
+              </a:gradFill>
+              <a:ln w="95250">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="4"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:gradFill flip="none" rotWithShape="1">
+                <a:gsLst>
+                  <a:gs pos="20000">
+                    <a:schemeClr val="accent5">
+                      <a:lumMod val="60000"/>
+                      <a:lumOff val="40000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="70000">
+                    <a:schemeClr val="accent5">
+                      <a:lumMod val="75000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="10800000" scaled="1"/>
+                <a:tileRect/>
+              </a:gradFill>
+              <a:ln w="95250">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="5"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:gradFill flip="none" rotWithShape="1">
+                <a:gsLst>
+                  <a:gs pos="20000">
+                    <a:schemeClr val="accent5">
+                      <a:lumMod val="60000"/>
+                      <a:lumOff val="40000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="70000">
+                    <a:schemeClr val="accent5">
+                      <a:lumMod val="75000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="10800000" scaled="1"/>
+                <a:tileRect/>
+              </a:gradFill>
+              <a:ln w="95250">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="6"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:gradFill flip="none" rotWithShape="1">
+                <a:gsLst>
+                  <a:gs pos="20000">
+                    <a:schemeClr val="accent5">
+                      <a:lumMod val="60000"/>
+                      <a:lumOff val="40000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="70000">
+                    <a:schemeClr val="accent5">
+                      <a:lumMod val="75000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="10800000" scaled="1"/>
+                <a:tileRect/>
+              </a:gradFill>
+              <a:ln w="95250">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="7"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:gradFill flip="none" rotWithShape="1">
+                <a:gsLst>
+                  <a:gs pos="20000">
+                    <a:schemeClr val="accent5">
+                      <a:lumMod val="60000"/>
+                      <a:lumOff val="40000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="70000">
+                    <a:schemeClr val="accent5">
+                      <a:lumMod val="75000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="10800000" scaled="1"/>
+                <a:tileRect/>
+              </a:gradFill>
+              <a:ln w="95250">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="8"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:gradFill flip="none" rotWithShape="1">
+                <a:gsLst>
+                  <a:gs pos="20000">
+                    <a:schemeClr val="accent5">
+                      <a:lumMod val="60000"/>
+                      <a:lumOff val="40000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="70000">
+                    <a:schemeClr val="accent5">
+                      <a:lumMod val="75000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="10800000" scaled="1"/>
+                <a:tileRect/>
+              </a:gradFill>
+              <a:ln w="95250">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="9"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:gradFill flip="none" rotWithShape="1">
+                <a:gsLst>
+                  <a:gs pos="20000">
+                    <a:schemeClr val="accent5">
+                      <a:lumMod val="60000"/>
+                      <a:lumOff val="40000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="70000">
+                    <a:schemeClr val="accent5">
+                      <a:lumMod val="75000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="10800000" scaled="1"/>
+                <a:tileRect/>
+              </a:gradFill>
+              <a:ln w="95250">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="10"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:gradFill flip="none" rotWithShape="1">
+                <a:gsLst>
+                  <a:gs pos="20000">
+                    <a:schemeClr val="accent5">
+                      <a:lumMod val="60000"/>
+                      <a:lumOff val="40000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="70000">
+                    <a:schemeClr val="accent5">
+                      <a:lumMod val="75000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="10800000" scaled="1"/>
+                <a:tileRect/>
+              </a:gradFill>
+              <a:ln w="95250">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="11"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:gradFill flip="none" rotWithShape="1">
+                <a:gsLst>
+                  <a:gs pos="20000">
+                    <a:schemeClr val="accent5">
+                      <a:lumMod val="60000"/>
+                      <a:lumOff val="40000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="70000">
+                    <a:schemeClr val="accent5">
+                      <a:lumMod val="75000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="10800000" scaled="1"/>
+                <a:tileRect/>
+              </a:gradFill>
+              <a:ln w="95250">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="12"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:gradFill flip="none" rotWithShape="1">
+                <a:gsLst>
+                  <a:gs pos="20000">
+                    <a:schemeClr val="accent5">
+                      <a:lumMod val="60000"/>
+                      <a:lumOff val="40000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="70000">
+                    <a:schemeClr val="accent5">
+                      <a:lumMod val="75000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="10800000" scaled="1"/>
+                <a:tileRect/>
+              </a:gradFill>
+              <a:ln w="95250">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="13"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:gradFill flip="none" rotWithShape="1">
+                <a:gsLst>
+                  <a:gs pos="20000">
+                    <a:schemeClr val="accent5">
+                      <a:lumMod val="60000"/>
+                      <a:lumOff val="40000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="70000">
+                    <a:schemeClr val="accent5">
+                      <a:lumMod val="75000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="10800000" scaled="1"/>
+                <a:tileRect/>
+              </a:gradFill>
+              <a:ln w="95250">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="14"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:gradFill flip="none" rotWithShape="1">
+                <a:gsLst>
+                  <a:gs pos="20000">
+                    <a:schemeClr val="accent5">
+                      <a:lumMod val="60000"/>
+                      <a:lumOff val="40000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="70000">
+                    <a:schemeClr val="accent5">
+                      <a:lumMod val="75000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="10800000" scaled="1"/>
+                <a:tileRect/>
+              </a:gradFill>
+              <a:ln w="95250">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="15"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:gradFill flip="none" rotWithShape="1">
+                <a:gsLst>
+                  <a:gs pos="20000">
+                    <a:schemeClr val="accent5">
+                      <a:lumMod val="60000"/>
+                      <a:lumOff val="40000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="70000">
+                    <a:schemeClr val="accent5">
+                      <a:lumMod val="75000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="10800000" scaled="1"/>
+                <a:tileRect/>
+              </a:gradFill>
+              <a:ln w="95250">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="16"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:gradFill flip="none" rotWithShape="1">
+                <a:gsLst>
+                  <a:gs pos="20000">
+                    <a:schemeClr val="accent5">
+                      <a:lumMod val="60000"/>
+                      <a:lumOff val="40000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="70000">
+                    <a:schemeClr val="accent5">
+                      <a:lumMod val="75000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="10800000" scaled="1"/>
+                <a:tileRect/>
+              </a:gradFill>
+              <a:ln w="95250">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="17"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:gradFill flip="none" rotWithShape="1">
+                <a:gsLst>
+                  <a:gs pos="20000">
+                    <a:schemeClr val="accent5">
+                      <a:lumMod val="60000"/>
+                      <a:lumOff val="40000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="70000">
+                    <a:schemeClr val="accent5">
+                      <a:lumMod val="75000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="10800000" scaled="1"/>
+                <a:tileRect/>
+              </a:gradFill>
+              <a:ln w="95250">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="18"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:gradFill flip="none" rotWithShape="1">
+                <a:gsLst>
+                  <a:gs pos="20000">
+                    <a:schemeClr val="accent5">
+                      <a:lumMod val="60000"/>
+                      <a:lumOff val="40000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="70000">
+                    <a:schemeClr val="accent5">
+                      <a:lumMod val="75000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="10800000" scaled="1"/>
+                <a:tileRect/>
+              </a:gradFill>
+              <a:ln w="95250">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="19"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:gradFill flip="none" rotWithShape="1">
+                <a:gsLst>
+                  <a:gs pos="20000">
+                    <a:schemeClr val="accent5">
+                      <a:lumMod val="60000"/>
+                      <a:lumOff val="40000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="70000">
+                    <a:schemeClr val="accent5">
+                      <a:lumMod val="75000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="10800000" scaled="1"/>
+                <a:tileRect/>
+              </a:gradFill>
+              <a:ln w="95250">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="20"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:gradFill flip="none" rotWithShape="1">
+                <a:gsLst>
+                  <a:gs pos="20000">
+                    <a:schemeClr val="accent5">
+                      <a:lumMod val="60000"/>
+                      <a:lumOff val="40000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="70000">
+                    <a:schemeClr val="accent5">
+                      <a:lumMod val="75000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="10800000" scaled="1"/>
+                <a:tileRect/>
+              </a:gradFill>
+              <a:ln w="95250">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="21"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:gradFill flip="none" rotWithShape="1">
+                <a:gsLst>
+                  <a:gs pos="20000">
+                    <a:schemeClr val="accent5">
+                      <a:lumMod val="60000"/>
+                      <a:lumOff val="40000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="70000">
+                    <a:schemeClr val="accent5">
+                      <a:lumMod val="75000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="10800000" scaled="1"/>
+                <a:tileRect/>
+              </a:gradFill>
+              <a:ln w="95250">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="22"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:gradFill flip="none" rotWithShape="1">
+                <a:gsLst>
+                  <a:gs pos="20000">
+                    <a:schemeClr val="accent5">
+                      <a:lumMod val="60000"/>
+                      <a:lumOff val="40000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="70000">
+                    <a:schemeClr val="accent5">
+                      <a:lumMod val="75000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="10800000" scaled="1"/>
+                <a:tileRect/>
+              </a:gradFill>
+              <a:ln w="95250">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="23"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:gradFill flip="none" rotWithShape="1">
+                <a:gsLst>
+                  <a:gs pos="20000">
+                    <a:schemeClr val="accent5">
+                      <a:lumMod val="60000"/>
+                      <a:lumOff val="40000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="70000">
+                    <a:schemeClr val="accent5">
+                      <a:lumMod val="75000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="10800000" scaled="1"/>
+                <a:tileRect/>
+              </a:gradFill>
+              <a:ln w="95250">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="24"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:gradFill flip="none" rotWithShape="1">
+                <a:gsLst>
+                  <a:gs pos="20000">
+                    <a:schemeClr val="accent5">
+                      <a:lumMod val="60000"/>
+                      <a:lumOff val="40000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="70000">
+                    <a:schemeClr val="accent5">
+                      <a:lumMod val="75000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="10800000" scaled="1"/>
+                <a:tileRect/>
+              </a:gradFill>
+              <a:ln w="95250">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="25"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:gradFill flip="none" rotWithShape="1">
+                <a:gsLst>
+                  <a:gs pos="20000">
+                    <a:schemeClr val="accent5">
+                      <a:lumMod val="60000"/>
+                      <a:lumOff val="40000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="70000">
+                    <a:schemeClr val="accent5">
+                      <a:lumMod val="75000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="10800000" scaled="1"/>
+                <a:tileRect/>
+              </a:gradFill>
+              <a:ln w="95250">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="26"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:gradFill flip="none" rotWithShape="1">
+                <a:gsLst>
+                  <a:gs pos="20000">
+                    <a:schemeClr val="accent5">
+                      <a:lumMod val="60000"/>
+                      <a:lumOff val="40000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="70000">
+                    <a:schemeClr val="accent5">
+                      <a:lumMod val="75000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="10800000" scaled="1"/>
+                <a:tileRect/>
+              </a:gradFill>
+              <a:ln w="95250">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="27"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:gradFill flip="none" rotWithShape="1">
+                <a:gsLst>
+                  <a:gs pos="20000">
+                    <a:schemeClr val="accent5">
+                      <a:lumMod val="60000"/>
+                      <a:lumOff val="40000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="70000">
+                    <a:schemeClr val="accent5">
+                      <a:lumMod val="75000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="10800000" scaled="1"/>
+                <a:tileRect/>
+              </a:gradFill>
+              <a:ln w="95250">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="28"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:gradFill flip="none" rotWithShape="1">
+                <a:gsLst>
+                  <a:gs pos="20000">
+                    <a:schemeClr val="accent5">
+                      <a:lumMod val="60000"/>
+                      <a:lumOff val="40000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="70000">
+                    <a:schemeClr val="accent5">
+                      <a:lumMod val="75000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="10800000" scaled="1"/>
+                <a:tileRect/>
+              </a:gradFill>
+              <a:ln w="95250">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="29"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:gradFill flip="none" rotWithShape="1">
+                <a:gsLst>
+                  <a:gs pos="20000">
+                    <a:schemeClr val="accent5">
+                      <a:lumMod val="60000"/>
+                      <a:lumOff val="40000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="70000">
+                    <a:schemeClr val="accent5">
+                      <a:lumMod val="75000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="10800000" scaled="1"/>
+                <a:tileRect/>
+              </a:gradFill>
+              <a:ln w="95250">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="30"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:gradFill flip="none" rotWithShape="1">
+                <a:gsLst>
+                  <a:gs pos="20000">
+                    <a:schemeClr val="accent5">
+                      <a:lumMod val="60000"/>
+                      <a:lumOff val="40000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="70000">
+                    <a:schemeClr val="accent5">
+                      <a:lumMod val="75000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="10800000" scaled="1"/>
+                <a:tileRect/>
+              </a:gradFill>
+              <a:ln w="95250">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="31"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:gradFill flip="none" rotWithShape="1">
+                <a:gsLst>
+                  <a:gs pos="20000">
+                    <a:schemeClr val="accent5">
+                      <a:lumMod val="60000"/>
+                      <a:lumOff val="40000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="70000">
+                    <a:schemeClr val="accent5">
+                      <a:lumMod val="75000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="10800000" scaled="1"/>
+                <a:tileRect/>
+              </a:gradFill>
+              <a:ln w="95250">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="32"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:gradFill flip="none" rotWithShape="1">
+                <a:gsLst>
+                  <a:gs pos="20000">
+                    <a:schemeClr val="accent5">
+                      <a:lumMod val="60000"/>
+                      <a:lumOff val="40000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="70000">
+                    <a:schemeClr val="accent5">
+                      <a:lumMod val="75000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="10800000" scaled="1"/>
+                <a:tileRect/>
+              </a:gradFill>
+              <a:ln w="95250">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="33"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:gradFill flip="none" rotWithShape="1">
+                <a:gsLst>
+                  <a:gs pos="20000">
+                    <a:schemeClr val="accent5">
+                      <a:lumMod val="60000"/>
+                      <a:lumOff val="40000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="70000">
+                    <a:schemeClr val="accent5">
+                      <a:lumMod val="75000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="10800000" scaled="1"/>
+                <a:tileRect/>
+              </a:gradFill>
+              <a:ln w="95250">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="34"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:gradFill flip="none" rotWithShape="1">
+                <a:gsLst>
+                  <a:gs pos="20000">
+                    <a:schemeClr val="accent5">
+                      <a:lumMod val="60000"/>
+                      <a:lumOff val="40000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="70000">
+                    <a:schemeClr val="accent5">
+                      <a:lumMod val="75000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="10800000" scaled="1"/>
+                <a:tileRect/>
+              </a:gradFill>
+              <a:ln w="95250">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="35"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:gradFill flip="none" rotWithShape="1">
+                <a:gsLst>
+                  <a:gs pos="20000">
+                    <a:schemeClr val="accent5">
+                      <a:lumMod val="60000"/>
+                      <a:lumOff val="40000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="70000">
+                    <a:schemeClr val="accent5">
+                      <a:lumMod val="75000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="10800000" scaled="1"/>
+                <a:tileRect/>
+              </a:gradFill>
+              <a:ln w="95250">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="36"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:gradFill flip="none" rotWithShape="1">
+                <a:gsLst>
+                  <a:gs pos="20000">
+                    <a:schemeClr val="accent5">
+                      <a:lumMod val="60000"/>
+                      <a:lumOff val="40000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="70000">
+                    <a:schemeClr val="accent5">
+                      <a:lumMod val="75000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="10800000" scaled="1"/>
+                <a:tileRect/>
+              </a:gradFill>
+              <a:ln w="95250">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="37"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:gradFill flip="none" rotWithShape="1">
+                <a:gsLst>
+                  <a:gs pos="20000">
+                    <a:schemeClr val="accent5">
+                      <a:lumMod val="60000"/>
+                      <a:lumOff val="40000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="70000">
+                    <a:schemeClr val="accent5">
+                      <a:lumMod val="75000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="10800000" scaled="1"/>
+                <a:tileRect/>
+              </a:gradFill>
+              <a:ln w="95250">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="38"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:gradFill flip="none" rotWithShape="1">
+                <a:gsLst>
+                  <a:gs pos="20000">
+                    <a:schemeClr val="accent5">
+                      <a:lumMod val="60000"/>
+                      <a:lumOff val="40000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="70000">
+                    <a:schemeClr val="accent5">
+                      <a:lumMod val="75000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="10800000" scaled="1"/>
+                <a:tileRect/>
+              </a:gradFill>
+              <a:ln w="95250">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="39"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:gradFill flip="none" rotWithShape="1">
+                <a:gsLst>
+                  <a:gs pos="20000">
+                    <a:schemeClr val="accent5">
+                      <a:lumMod val="60000"/>
+                      <a:lumOff val="40000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="70000">
+                    <a:schemeClr val="accent5">
+                      <a:lumMod val="75000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="10800000" scaled="1"/>
+                <a:tileRect/>
+              </a:gradFill>
+              <a:ln w="95250">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="40"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:gradFill flip="none" rotWithShape="1">
+                <a:gsLst>
+                  <a:gs pos="20000">
+                    <a:schemeClr val="accent5">
+                      <a:lumMod val="60000"/>
+                      <a:lumOff val="40000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="70000">
+                    <a:schemeClr val="accent5">
+                      <a:lumMod val="75000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="10800000" scaled="1"/>
+                <a:tileRect/>
+              </a:gradFill>
+              <a:ln w="95250">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="41"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:gradFill flip="none" rotWithShape="1">
+                <a:gsLst>
+                  <a:gs pos="20000">
+                    <a:schemeClr val="accent5">
+                      <a:lumMod val="60000"/>
+                      <a:lumOff val="40000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="70000">
+                    <a:schemeClr val="accent5">
+                      <a:lumMod val="75000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="10800000" scaled="1"/>
+                <a:tileRect/>
+              </a:gradFill>
+              <a:ln w="95250">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="42"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:gradFill flip="none" rotWithShape="1">
+                <a:gsLst>
+                  <a:gs pos="20000">
+                    <a:schemeClr val="accent5">
+                      <a:lumMod val="60000"/>
+                      <a:lumOff val="40000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="70000">
+                    <a:schemeClr val="accent5">
+                      <a:lumMod val="75000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="10800000" scaled="1"/>
+                <a:tileRect/>
+              </a:gradFill>
+              <a:ln w="95250">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="43"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:gradFill flip="none" rotWithShape="1">
+                <a:gsLst>
+                  <a:gs pos="20000">
+                    <a:schemeClr val="accent5">
+                      <a:lumMod val="60000"/>
+                      <a:lumOff val="40000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="70000">
+                    <a:schemeClr val="accent5">
+                      <a:lumMod val="75000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="10800000" scaled="1"/>
+                <a:tileRect/>
+              </a:gradFill>
+              <a:ln w="95250">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="44"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:gradFill flip="none" rotWithShape="1">
+                <a:gsLst>
+                  <a:gs pos="20000">
+                    <a:schemeClr val="accent5">
+                      <a:lumMod val="60000"/>
+                      <a:lumOff val="40000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="70000">
+                    <a:schemeClr val="accent5">
+                      <a:lumMod val="75000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="10800000" scaled="1"/>
+                <a:tileRect/>
+              </a:gradFill>
+              <a:ln w="95250">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="45"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:gradFill flip="none" rotWithShape="1">
+                <a:gsLst>
+                  <a:gs pos="20000">
+                    <a:schemeClr val="accent5">
+                      <a:lumMod val="60000"/>
+                      <a:lumOff val="40000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="70000">
+                    <a:schemeClr val="accent5">
+                      <a:lumMod val="75000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="10800000" scaled="1"/>
+                <a:tileRect/>
+              </a:gradFill>
+              <a:ln w="95250">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="46"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:gradFill flip="none" rotWithShape="1">
+                <a:gsLst>
+                  <a:gs pos="20000">
+                    <a:schemeClr val="accent5">
+                      <a:lumMod val="60000"/>
+                      <a:lumOff val="40000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="70000">
+                    <a:schemeClr val="accent5">
+                      <a:lumMod val="75000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="10800000" scaled="1"/>
+                <a:tileRect/>
+              </a:gradFill>
+              <a:ln w="95250">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="47"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:gradFill flip="none" rotWithShape="1">
+                <a:gsLst>
+                  <a:gs pos="20000">
+                    <a:schemeClr val="accent5">
+                      <a:lumMod val="60000"/>
+                      <a:lumOff val="40000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="70000">
+                    <a:schemeClr val="accent5">
+                      <a:lumMod val="75000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="10800000" scaled="1"/>
+                <a:tileRect/>
+              </a:gradFill>
+              <a:ln w="95250">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="48"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:gradFill flip="none" rotWithShape="1">
+                <a:gsLst>
+                  <a:gs pos="20000">
+                    <a:schemeClr val="accent5">
+                      <a:lumMod val="60000"/>
+                      <a:lumOff val="40000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="70000">
+                    <a:schemeClr val="accent5">
+                      <a:lumMod val="75000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="10800000" scaled="1"/>
+                <a:tileRect/>
+              </a:gradFill>
+              <a:ln w="95250">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="49"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:gradFill flip="none" rotWithShape="1">
+                <a:gsLst>
+                  <a:gs pos="20000">
+                    <a:schemeClr val="accent5">
+                      <a:lumMod val="60000"/>
+                      <a:lumOff val="40000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="70000">
+                    <a:schemeClr val="accent5">
+                      <a:lumMod val="75000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="10800000" scaled="1"/>
+                <a:tileRect/>
+              </a:gradFill>
+              <a:ln w="95250">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:val>
+            <c:numLit>
+              <c:formatCode>General</c:formatCode>
+              <c:ptCount val="50"/>
+              <c:pt idx="0">
+                <c:v>1</c:v>
+              </c:pt>
+              <c:pt idx="1">
+                <c:v>1</c:v>
+              </c:pt>
+              <c:pt idx="2">
+                <c:v>1</c:v>
+              </c:pt>
+              <c:pt idx="3">
+                <c:v>1</c:v>
+              </c:pt>
+              <c:pt idx="4">
+                <c:v>1</c:v>
+              </c:pt>
+              <c:pt idx="5">
+                <c:v>1</c:v>
+              </c:pt>
+              <c:pt idx="6">
+                <c:v>1</c:v>
+              </c:pt>
+              <c:pt idx="7">
+                <c:v>1</c:v>
+              </c:pt>
+              <c:pt idx="8">
+                <c:v>1</c:v>
+              </c:pt>
+              <c:pt idx="9">
+                <c:v>1</c:v>
+              </c:pt>
+              <c:pt idx="10">
+                <c:v>1</c:v>
+              </c:pt>
+              <c:pt idx="11">
+                <c:v>1</c:v>
+              </c:pt>
+              <c:pt idx="12">
+                <c:v>1</c:v>
+              </c:pt>
+              <c:pt idx="13">
+                <c:v>1</c:v>
+              </c:pt>
+              <c:pt idx="14">
+                <c:v>1</c:v>
+              </c:pt>
+              <c:pt idx="15">
+                <c:v>1</c:v>
+              </c:pt>
+              <c:pt idx="16">
+                <c:v>1</c:v>
+              </c:pt>
+              <c:pt idx="17">
+                <c:v>1</c:v>
+              </c:pt>
+              <c:pt idx="18">
+                <c:v>1</c:v>
+              </c:pt>
+              <c:pt idx="19">
+                <c:v>1</c:v>
+              </c:pt>
+              <c:pt idx="20">
+                <c:v>1</c:v>
+              </c:pt>
+              <c:pt idx="21">
+                <c:v>1</c:v>
+              </c:pt>
+              <c:pt idx="22">
+                <c:v>1</c:v>
+              </c:pt>
+              <c:pt idx="23">
+                <c:v>1</c:v>
+              </c:pt>
+              <c:pt idx="24">
+                <c:v>1</c:v>
+              </c:pt>
+              <c:pt idx="25">
+                <c:v>1</c:v>
+              </c:pt>
+              <c:pt idx="26">
+                <c:v>1</c:v>
+              </c:pt>
+              <c:pt idx="27">
+                <c:v>1</c:v>
+              </c:pt>
+              <c:pt idx="28">
+                <c:v>1</c:v>
+              </c:pt>
+              <c:pt idx="29">
+                <c:v>1</c:v>
+              </c:pt>
+              <c:pt idx="30">
+                <c:v>1</c:v>
+              </c:pt>
+              <c:pt idx="31">
+                <c:v>1</c:v>
+              </c:pt>
+              <c:pt idx="32">
+                <c:v>1</c:v>
+              </c:pt>
+              <c:pt idx="33">
+                <c:v>1</c:v>
+              </c:pt>
+              <c:pt idx="34">
+                <c:v>1</c:v>
+              </c:pt>
+              <c:pt idx="35">
+                <c:v>1</c:v>
+              </c:pt>
+              <c:pt idx="36">
+                <c:v>1</c:v>
+              </c:pt>
+              <c:pt idx="37">
+                <c:v>1</c:v>
+              </c:pt>
+              <c:pt idx="38">
+                <c:v>1</c:v>
+              </c:pt>
+              <c:pt idx="39">
+                <c:v>1</c:v>
+              </c:pt>
+              <c:pt idx="40">
+                <c:v>1</c:v>
+              </c:pt>
+              <c:pt idx="41">
+                <c:v>1</c:v>
+              </c:pt>
+              <c:pt idx="42">
+                <c:v>1</c:v>
+              </c:pt>
+              <c:pt idx="43">
+                <c:v>1</c:v>
+              </c:pt>
+              <c:pt idx="44">
+                <c:v>1</c:v>
+              </c:pt>
+              <c:pt idx="45">
+                <c:v>1</c:v>
+              </c:pt>
+              <c:pt idx="46">
+                <c:v>1</c:v>
+              </c:pt>
+              <c:pt idx="47">
+                <c:v>1</c:v>
+              </c:pt>
+              <c:pt idx="48">
+                <c:v>1</c:v>
+              </c:pt>
+              <c:pt idx="49">
+                <c:v>1</c:v>
+              </c:pt>
+            </c:numLit>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-6316-442F-9BDE-730853A04D41}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:showLeaderLines val="1"/>
+        </c:dLbls>
+        <c:firstSliceAng val="0"/>
+        <c:holeSize val="75"/>
+      </c:doughnutChart>
+      <c:pieChart>
+        <c:varyColors val="1"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>mask1</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="19050">
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000002-6316-442F-9BDE-730853A04D41}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="1"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:alpha val="78000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000003-6316-442F-9BDE-730853A04D41}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$3:$C$3</c:f>
+              <c:numCache>
+                <c:formatCode>0%</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>0.78</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.21999999999999997</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-6316-442F-9BDE-730853A04D41}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:showLeaderLines val="1"/>
+        </c:dLbls>
+        <c:firstSliceAng val="0"/>
+      </c:pieChart>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>ends</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst>
+              <a:glow rad="101600">
+                <a:schemeClr val="accent5">
+                  <a:lumMod val="75000"/>
+                </a:schemeClr>
+              </a:glow>
+            </a:effectLst>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="26"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="accent5">
+                    <a:lumMod val="75000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst>
+                <a:glow rad="101600">
+                  <a:schemeClr val="accent5">
+                    <a:lumMod val="75000"/>
+                  </a:schemeClr>
+                </a:glow>
+              </a:effectLst>
+            </c:spPr>
+          </c:marker>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:marker>
+              <c:symbol val="circle"/>
+              <c:size val="26"/>
+              <c:spPr>
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:ln w="9525">
+                  <a:gradFill>
+                    <a:gsLst>
+                      <a:gs pos="0">
+                        <a:srgbClr val="FFFF00"/>
+                      </a:gs>
+                      <a:gs pos="66000">
+                        <a:schemeClr val="accent4">
+                          <a:lumMod val="40000"/>
+                          <a:lumOff val="60000"/>
+                        </a:schemeClr>
+                      </a:gs>
+                    </a:gsLst>
+                    <a:lin ang="5400000" scaled="1"/>
+                  </a:gradFill>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+            </c:marker>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:ln w="25400" cap="rnd">
+                <a:noFill/>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000006-6316-442F-9BDE-730853A04D41}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="1"/>
+            <c:marker>
+              <c:symbol val="circle"/>
+              <c:size val="26"/>
+              <c:spPr>
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:ln w="19050">
+                  <a:gradFill>
+                    <a:gsLst>
+                      <a:gs pos="0">
+                        <a:schemeClr val="accent5">
+                          <a:lumMod val="60000"/>
+                          <a:lumOff val="40000"/>
+                        </a:schemeClr>
+                      </a:gs>
+                      <a:gs pos="45000">
+                        <a:schemeClr val="accent5">
+                          <a:lumMod val="50000"/>
+                        </a:schemeClr>
+                      </a:gs>
+                    </a:gsLst>
+                    <a:lin ang="5400000" scaled="1"/>
+                  </a:gradFill>
+                </a:ln>
+                <a:effectLst>
+                  <a:glow rad="63500">
+                    <a:schemeClr val="accent5">
+                      <a:satMod val="175000"/>
+                      <a:alpha val="40000"/>
+                    </a:schemeClr>
+                  </a:glow>
+                </a:effectLst>
+              </c:spPr>
+            </c:marker>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:ln w="25400" cap="rnd">
+                <a:noFill/>
+                <a:round/>
+              </a:ln>
+              <a:effectLst>
+                <a:glow rad="63500">
+                  <a:schemeClr val="accent5">
+                    <a:satMod val="175000"/>
+                    <a:alpha val="40000"/>
+                  </a:schemeClr>
+                </a:glow>
+              </a:effectLst>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000005-6316-442F-9BDE-730853A04D41}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="0"/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:fld id="{20D0675F-84F3-4DFC-8C8C-A0B7F98D61F9}" type="CELLRANGE">
+                      <a:rPr lang="en-US"/>
+                      <a:pPr/>
+                      <a:t>[CELLRANGE]</a:t>
+                    </a:fld>
+                    <a:endParaRPr lang="en-US"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:dLblPos val="ctr"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
+                  <c15:showDataLabelsRange val="1"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000006-6316-442F-9BDE-730853A04D41}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="1"/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:fld id="{7FB72707-F8F8-4EE6-AC62-4D926BAE2135}" type="CELLRANGE">
+                      <a:rPr lang="en-US"/>
+                      <a:pPr/>
+                      <a:t>[CELLRANGE]</a:t>
+                    </a:fld>
+                    <a:endParaRPr lang="en-US"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:dLblPos val="ctr"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
+                  <c15:showDataLabelsRange val="1"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000005-6316-442F-9BDE-730853A04D41}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="bg1"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="ctr"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showDataLabelsRange val="1"/>
+                <c15:showLeaderLines val="0"/>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$E$3:$E$4</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-0.98228725072868861</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$F$3:$F$4</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.18738131458572493</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+              <c15:datalabelsRange>
+                <c15:f>Sheet1!$H$3:$H$4</c15:f>
+                <c15:dlblRangeCache>
+                  <c:ptCount val="2"/>
+                  <c:pt idx="0">
+                    <c:v>22%</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>78%</c:v>
+                  </c:pt>
+                </c15:dlblRangeCache>
+              </c15:datalabelsRange>
+            </c:ext>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000004-6316-442F-9BDE-730853A04D41}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1431395327"/>
+        <c:axId val="1431396575"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="1431396575"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="1.1500000000000001"/>
+          <c:min val="-1.1500000000000001"/>
+        </c:scaling>
+        <c:delete val="1"/>
+        <c:axPos val="l"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="1431395327"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1431395327"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="1.1500000000000001"/>
+          <c:min val="-1.1500000000000001"/>
+        </c:scaling>
+        <c:delete val="1"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="1431396575"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln w="25400">
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="tx1"/>
+    </a:solidFill>
     <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
       <a:solidFill>
         <a:schemeClr val="tx1">
@@ -5352,6 +8234,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors7.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="251">
   <cs:axisTitle>
@@ -8452,20 +11374,539 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style7.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="251">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="25400">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>42862</xdr:colOff>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>519112</xdr:colOff>
       <xdr:row>7</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
+      <xdr:rowOff>47625</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>171450</xdr:colOff>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>342900</xdr:colOff>
       <xdr:row>22</xdr:row>
-      <xdr:rowOff>95250</xdr:rowOff>
+      <xdr:rowOff>104775</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -8655,7 +12096,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="5867400" y="5476875"/>
+          <a:off x="6105525" y="5476875"/>
           <a:ext cx="1071384" cy="718466"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -8691,7 +12132,8 @@
               <a:latin typeface="Calibri"/>
               <a:cs typeface="Calibri"/>
             </a:rPr>
-            <a:t>67%</a:t>
+            <a:pPr/>
+            <a:t>78%</a:t>
           </a:fld>
           <a:endParaRPr lang="en-US" sz="4000">
             <a:solidFill>
@@ -8707,12 +12149,12 @@
     <xdr:from>
       <xdr:col>12</xdr:col>
       <xdr:colOff>366712</xdr:colOff>
-      <xdr:row>24</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>20</xdr:col>
-      <xdr:colOff>61912</xdr:colOff>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>247650</xdr:colOff>
       <xdr:row>38</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
@@ -8734,6 +12176,42 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId6"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>180975</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>400050</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="11" name="Chart 10">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{13290B57-1070-71FE-8626-1B88CE9BD19D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId7"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -8785,7 +12263,8 @@
               <a:latin typeface="Calibri"/>
               <a:cs typeface="Calibri"/>
             </a:rPr>
-            <a:t>67%</a:t>
+            <a:pPr/>
+            <a:t>78%</a:t>
           </a:fld>
           <a:endParaRPr lang="en-US" sz="4000">
             <a:solidFill>
@@ -9096,10 +12575,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{89EC5DBB-5C92-4094-8D89-A11E4D0B3EC1}">
-  <dimension ref="A2:C4"/>
+  <dimension ref="A2:H4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9107,9 +12586,10 @@
     <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -9119,22 +12599,53 @@
       <c r="C2" s="4" t="s">
         <v>3</v>
       </c>
+      <c r="E2" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="F2" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>6</v>
+      </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>0</v>
       </c>
       <c r="B3" s="1">
-        <v>0.67</v>
+        <v>0.78</v>
       </c>
       <c r="C3" s="1">
         <f>1-B3</f>
-        <v>0.32999999999999996</v>
+        <v>0.21999999999999997</v>
+      </c>
+      <c r="E3" s="5">
+        <v>0</v>
+      </c>
+      <c r="F3" s="5">
+        <v>1</v>
+      </c>
+      <c r="H3" s="6">
+        <f>C3</f>
+        <v>0.21999999999999997</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
+      <c r="E4">
+        <f>-SIN(C3*2*PI())</f>
+        <v>-0.98228725072868861</v>
+      </c>
+      <c r="F4">
+        <f>COS(C3*2*PI())</f>
+        <v>0.18738131458572493</v>
+      </c>
+      <c r="H4" s="6">
+        <f>B3</f>
+        <v>0.78</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>